<commit_message>
Add level scaling value
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -121,6 +121,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">プレイヤーレベルに基づいて魚をレベルアップする機能を有効または無効にします。
 </t>
@@ -139,6 +140,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">に設定するとレベルアップが有効になり、</t>
     </r>
@@ -156,6 +158,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">に設定すると無効になります。</t>
     </r>
@@ -166,6 +169,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">启用或禁用根据玩家等级提升鱼的等级。
 设置为 </t>
@@ -184,6 +188,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">启用等级调整，或设置为 </t>
     </r>
@@ -201,6 +206,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">禁用此功能。</t>
     </r>
@@ -222,63 +228,51 @@
   </si>
   <si>
     <t xml:space="preserve">Enable or disable vanilla-style scaling for fishing level.
-When enabled, fishing level is divided by 10 for more balanced quality and level adjustments.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">釣りレベルのスケーリングをバニラ風に調整する機能を有効または無効にします。
-有効にすると、釣りレベルは</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">で割られ、品質やレベルの上昇がより抑えられます。</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">启用或禁用类似原版的钓鱼等级缩放。
-启用后，钓鱼等级将除以</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">，以实现更平衡的质量和等级调整。</t>
-    </r>
+When enabled, fishing level is divided by the configured Level Scaling value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">釣りレベルのスケーリングをバニラ風に調整する機能を有効または無効にします。
+有効にすると、釣りレベルが設定されたスケーリング除数で割られ、品質やレベルの上昇がより抑えられます。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用或禁用类似原版的钓鱼等级缩放。
+启用后，钓鱼等级将根据配置的缩放除数进行缩放，以实现更平衡的质量和等级调整。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level Scaling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">レベルスケーリング</t>
+  </si>
+  <si>
+    <t xml:space="preserve">等级缩放</t>
+  </si>
+  <si>
+    <t xml:space="preserve">topic01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level Scaling Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">レベルスケーリング値</t>
+  </si>
+  <si>
+    <t xml:space="preserve">等级缩放数值</t>
+  </si>
+  <si>
+    <t xml:space="preserve">topic02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slider Step</t>
+  </si>
+  <si>
+    <t xml:space="preserve">スライダーのステップ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">滑块步长</t>
   </si>
 </sst>
 </file>
@@ -288,7 +282,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -313,6 +307,12 @@
     <font>
       <sz val="10"/>
       <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Noto Sans SC"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -364,7 +364,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -383,6 +383,14 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -508,10 +516,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -663,6 +671,48 @@
         <v>39</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>